<commit_message>
changed ticks to reflect each magnitude
</commit_message>
<xml_diff>
--- a/Data/event_list_union.xlsx
+++ b/Data/event_list_union.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>GOES Proton Event Detector List</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -48,16 +52,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -65,8 +97,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -90,11 +137,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -106,6 +169,8 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -117,6 +182,8 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,404 +513,421 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H28"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="J4" sqref="J4:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="2" spans="1:8">
-      <c r="B2">
+    <row r="1" spans="1:6" ht="18">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="D2" s="3">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="E2" s="3">
         <v>3</v>
       </c>
-      <c r="G2">
+      <c r="F2" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
+    <row r="3" spans="1:6">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>20110321</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>20110607</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20110608</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>20110804</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>20110809</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>20110907</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>20120123</v>
+      </c>
+      <c r="C8" s="2">
+        <v>20120124</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>20120127</v>
+      </c>
+      <c r="C9" s="2">
+        <v>20120128</v>
+      </c>
+      <c r="D9" s="2">
+        <v>20120129</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>20120307</v>
+      </c>
+      <c r="C10" s="2">
+        <v>20120308</v>
+      </c>
+      <c r="D10" s="2">
+        <v>20120309</v>
+      </c>
+      <c r="E10" s="2">
+        <v>20120310</v>
+      </c>
+      <c r="F10" s="2">
+        <v>20120311</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>20120313</v>
+      </c>
+      <c r="C11" s="2">
+        <v>20120314</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>20120517</v>
+      </c>
+      <c r="C12" s="2">
+        <v>20120518</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="4">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>20120707</v>
+      </c>
+      <c r="C13" s="2">
+        <v>20120708</v>
+      </c>
+      <c r="D13" s="2">
+        <v>20120709</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>20120712</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>20120719</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="D3">
+      <c r="B16" s="2">
         <v>20120723</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>20110607</v>
-      </c>
-      <c r="C4">
+      <c r="C16" s="2">
+        <v>20120724</v>
+      </c>
+      <c r="D16" s="2">
+        <v>20120725</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="B17" s="2">
         <v>20130411</v>
       </c>
-      <c r="E4">
-        <v>20110608</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>20110804</v>
-      </c>
-      <c r="C5">
+      <c r="C17" s="2">
+        <v>20130412</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="D5">
+      <c r="B18" s="2">
         <v>20130522</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>20110809</v>
-      </c>
-      <c r="C6">
+      <c r="C18" s="2">
+        <v>20130523</v>
+      </c>
+      <c r="D18" s="2">
+        <v>20130524</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="D6">
+      <c r="B19" s="2">
         <v>20131102</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>20110907</v>
-      </c>
-      <c r="C7">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="D7">
+      <c r="B20" s="2">
         <v>20131228</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>20120123</v>
-      </c>
-      <c r="C8">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="D8">
+      <c r="B21" s="2">
         <v>20140106</v>
       </c>
-      <c r="E8">
-        <v>20120124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>20120127</v>
-      </c>
-      <c r="C9">
+      <c r="C21" s="2">
+        <v>20140107</v>
+      </c>
+      <c r="D21" s="2">
+        <v>20140108</v>
+      </c>
+      <c r="E21" s="2">
+        <v>20140109</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="D9">
+      <c r="B22" s="2">
         <v>20140220</v>
       </c>
-      <c r="E9">
-        <v>20120128</v>
-      </c>
-      <c r="F9">
-        <v>20120129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>20120307</v>
-      </c>
-      <c r="C10">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="D10">
+      <c r="B23" s="2">
         <v>20140225</v>
       </c>
-      <c r="E10">
-        <v>20120308</v>
-      </c>
-      <c r="F10">
-        <v>20120309</v>
-      </c>
-      <c r="G10">
-        <v>20120310</v>
-      </c>
-      <c r="H10">
-        <v>20120311</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>20120313</v>
-      </c>
-      <c r="C11">
+      <c r="C23" s="2">
+        <v>20140226</v>
+      </c>
+      <c r="D23" s="2">
+        <v>20140227</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="D11">
+      <c r="B24" s="2">
         <v>20140418</v>
       </c>
-      <c r="E11">
-        <v>20120314</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>20120517</v>
-      </c>
-      <c r="C12">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="D12">
+      <c r="B25" s="2">
         <v>20140902</v>
       </c>
-      <c r="E12">
-        <v>20120518</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>20120707</v>
-      </c>
-      <c r="C13">
+      <c r="C25" s="2">
+        <v>20140903</v>
+      </c>
+      <c r="D25" s="2">
+        <v>20140904</v>
+      </c>
+      <c r="E25" s="2">
+        <v>20140905</v>
+      </c>
+      <c r="F25" s="2">
+        <v>20140906</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="4">
         <v>24</v>
       </c>
-      <c r="D13">
+      <c r="B26" s="2">
         <v>20140910</v>
       </c>
-      <c r="E13">
-        <v>20120708</v>
-      </c>
-      <c r="F13">
-        <v>20120709</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>20120712</v>
-      </c>
-      <c r="C14">
+      <c r="C26" s="2">
+        <v>20140911</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="4">
         <v>25</v>
       </c>
-      <c r="D14">
+      <c r="B27" s="2">
         <v>20151029</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>20120719</v>
-      </c>
-      <c r="C15">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="4">
         <v>26</v>
       </c>
-      <c r="D15">
+      <c r="B28" s="2">
         <v>20170906</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>20120723</v>
-      </c>
-      <c r="E16">
-        <v>20120724</v>
-      </c>
-      <c r="F16">
-        <v>20120725</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>20130411</v>
-      </c>
-      <c r="E17">
-        <v>20130412</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>20130522</v>
-      </c>
-      <c r="E18">
-        <v>20130523</v>
-      </c>
-      <c r="F18">
-        <v>20130524</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>20131102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>20131228</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>20140106</v>
-      </c>
-      <c r="E21">
-        <v>20140107</v>
-      </c>
-      <c r="F21">
-        <v>20140108</v>
-      </c>
-      <c r="G21">
-        <v>20140109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>20140220</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23">
-        <v>20140225</v>
-      </c>
-      <c r="E23">
-        <v>20140226</v>
-      </c>
-      <c r="F23">
-        <v>20140227</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24">
-        <v>20140418</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25">
-        <v>20140902</v>
-      </c>
-      <c r="E25">
-        <v>20140903</v>
-      </c>
-      <c r="F25">
-        <v>20140904</v>
-      </c>
-      <c r="G25">
-        <v>20140905</v>
-      </c>
-      <c r="H25">
-        <v>20140906</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>20140910</v>
-      </c>
-      <c r="E26">
-        <v>20140911</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27">
-        <v>20151029</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>20170906</v>
-      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
readme changes and deprecated scripts
</commit_message>
<xml_diff>
--- a/Data/event_list_union.xlsx
+++ b/Data/event_list_union.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,16 +20,121 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="36">
   <si>
     <t>GOES Proton Event Detector List</t>
+  </si>
+  <si>
+    <t>X1.5</t>
+  </si>
+  <si>
+    <t>'1'</t>
+  </si>
+  <si>
+    <t>'2'</t>
+  </si>
+  <si>
+    <t>'4'</t>
+  </si>
+  <si>
+    <t>'5'</t>
+  </si>
+  <si>
+    <t>X6.9</t>
+  </si>
+  <si>
+    <t>'full'</t>
+  </si>
+  <si>
+    <t>X2.1</t>
+  </si>
+  <si>
+    <t>X1.4</t>
+  </si>
+  <si>
+    <t>X1.9</t>
+  </si>
+  <si>
+    <t>X1.7</t>
+  </si>
+  <si>
+    <t>X5.4</t>
+  </si>
+  <si>
+    <t>X1.3</t>
+  </si>
+  <si>
+    <t>X1.1</t>
+  </si>
+  <si>
+    <t>X1.8</t>
+  </si>
+  <si>
+    <t>X2.8</t>
+  </si>
+  <si>
+    <t>X3.2</t>
+  </si>
+  <si>
+    <t>X1.2</t>
+  </si>
+  <si>
+    <t>X1.0</t>
+  </si>
+  <si>
+    <t>X2.3</t>
+  </si>
+  <si>
+    <t>X3.3</t>
+  </si>
+  <si>
+    <t>X4.9</t>
+  </si>
+  <si>
+    <t>X2.2</t>
+  </si>
+  <si>
+    <t>X1.6</t>
+  </si>
+  <si>
+    <t>X3.1</t>
+  </si>
+  <si>
+    <t>X2.0</t>
+  </si>
+  <si>
+    <t>X2.7</t>
+  </si>
+  <si>
+    <t>full'</t>
+  </si>
+  <si>
+    <t>X-Flare List</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Flare Class</t>
+  </si>
+  <si>
+    <t>Start Hour</t>
+  </si>
+  <si>
+    <t>End Hour</t>
+  </si>
+  <si>
+    <t>no data in goes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,8 +174,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,6 +198,66 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -113,7 +286,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -141,8 +314,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -156,8 +335,41 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -171,6 +383,9 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -184,6 +399,9 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -518,8 +736,8 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:L17"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -931,4 +1149,1729 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="18">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="8">
+        <v>2011</v>
+      </c>
+      <c r="B3" s="13">
+        <v>20110309</v>
+      </c>
+      <c r="C3" s="13">
+        <v>20110310</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="13">
+        <v>23</v>
+      </c>
+      <c r="F3" s="13">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>13</v>
+      </c>
+      <c r="L3">
+        <v>15</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="8"/>
+      <c r="B4" s="13">
+        <v>20110809</v>
+      </c>
+      <c r="C4" s="13">
+        <v>20110809</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="13">
+        <v>7</v>
+      </c>
+      <c r="F4" s="13">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>13</v>
+      </c>
+      <c r="L4">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="8"/>
+      <c r="B5" s="13">
+        <v>20110906</v>
+      </c>
+      <c r="C5" s="13">
+        <v>20110907</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="13">
+        <v>22</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>13</v>
+      </c>
+      <c r="L5">
+        <v>15</v>
+      </c>
+      <c r="M5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="8"/>
+      <c r="B6" s="13">
+        <v>20110922</v>
+      </c>
+      <c r="C6" s="13">
+        <v>20110922</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="13">
+        <v>10</v>
+      </c>
+      <c r="F6" s="13">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>13</v>
+      </c>
+      <c r="L6">
+        <v>15</v>
+      </c>
+      <c r="M6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="8"/>
+      <c r="B7" s="13">
+        <v>20110924</v>
+      </c>
+      <c r="C7" s="13">
+        <v>20110924</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="13">
+        <v>9</v>
+      </c>
+      <c r="F7" s="13">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>13</v>
+      </c>
+      <c r="L7">
+        <v>15</v>
+      </c>
+      <c r="M7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="8"/>
+      <c r="B8" s="13">
+        <v>20111103</v>
+      </c>
+      <c r="C8" s="13">
+        <v>20111103</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="13">
+        <v>20</v>
+      </c>
+      <c r="F8" s="13">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>13</v>
+      </c>
+      <c r="L8">
+        <v>15</v>
+      </c>
+      <c r="M8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="9">
+        <v>2012</v>
+      </c>
+      <c r="B9" s="14">
+        <v>20120127</v>
+      </c>
+      <c r="C9" s="14">
+        <v>20120127</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="14">
+        <v>17</v>
+      </c>
+      <c r="F9" s="14">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>13</v>
+      </c>
+      <c r="L9">
+        <v>15</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="9"/>
+      <c r="B10" s="14">
+        <v>20120307</v>
+      </c>
+      <c r="C10" s="14">
+        <v>20120307</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0</v>
+      </c>
+      <c r="F10" s="14">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>13</v>
+      </c>
+      <c r="L10">
+        <v>15</v>
+      </c>
+      <c r="M10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="9"/>
+      <c r="B11" s="14">
+        <v>20120307</v>
+      </c>
+      <c r="C11" s="14">
+        <v>20120307</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="14">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>13</v>
+      </c>
+      <c r="L11">
+        <v>15</v>
+      </c>
+      <c r="M11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="9"/>
+      <c r="B12" s="14">
+        <v>20120706</v>
+      </c>
+      <c r="C12" s="14">
+        <v>20120707</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="14">
+        <v>23</v>
+      </c>
+      <c r="F12" s="14">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <v>13</v>
+      </c>
+      <c r="L12">
+        <v>15</v>
+      </c>
+      <c r="M12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="9"/>
+      <c r="B13" s="14">
+        <v>20120712</v>
+      </c>
+      <c r="C13" s="14">
+        <v>20120712</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="14">
+        <v>15</v>
+      </c>
+      <c r="F13" s="14">
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13">
+        <v>13</v>
+      </c>
+      <c r="L13">
+        <v>15</v>
+      </c>
+      <c r="M13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="9"/>
+      <c r="B14" s="14">
+        <v>20121023</v>
+      </c>
+      <c r="C14" s="14">
+        <v>20121023</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="14">
+        <v>3</v>
+      </c>
+      <c r="F14" s="14">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>13</v>
+      </c>
+      <c r="L14">
+        <v>15</v>
+      </c>
+      <c r="M14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="10">
+        <v>2013</v>
+      </c>
+      <c r="B15" s="15">
+        <v>20130513</v>
+      </c>
+      <c r="C15" s="15">
+        <v>20130513</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="15">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15">
+        <v>13</v>
+      </c>
+      <c r="L15">
+        <v>15</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="10"/>
+      <c r="B16" s="15">
+        <v>20130513</v>
+      </c>
+      <c r="C16" s="15">
+        <v>20130513</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="15">
+        <v>15</v>
+      </c>
+      <c r="F16" s="15">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16">
+        <v>13</v>
+      </c>
+      <c r="L16">
+        <v>15</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="10"/>
+      <c r="B17" s="15">
+        <v>20130514</v>
+      </c>
+      <c r="C17" s="15">
+        <v>20130514</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="15">
+        <v>0</v>
+      </c>
+      <c r="F17" s="15">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17">
+        <v>13</v>
+      </c>
+      <c r="L17">
+        <v>15</v>
+      </c>
+      <c r="M17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="10"/>
+      <c r="B18" s="15">
+        <v>20130515</v>
+      </c>
+      <c r="C18" s="15">
+        <v>20130515</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="15">
+        <v>1</v>
+      </c>
+      <c r="F18" s="15">
+        <v>4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>13</v>
+      </c>
+      <c r="L18">
+        <v>15</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="10"/>
+      <c r="B19" s="15">
+        <v>20131025</v>
+      </c>
+      <c r="C19" s="15">
+        <v>20131025</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="15">
+        <v>7</v>
+      </c>
+      <c r="F19" s="15">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19">
+        <v>13</v>
+      </c>
+      <c r="L19">
+        <v>15</v>
+      </c>
+      <c r="M19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="10"/>
+      <c r="B20" s="15">
+        <v>20131025</v>
+      </c>
+      <c r="C20" s="15">
+        <v>20131025</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="15">
+        <v>14</v>
+      </c>
+      <c r="F20" s="15">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20">
+        <v>13</v>
+      </c>
+      <c r="L20">
+        <v>15</v>
+      </c>
+      <c r="M20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="10"/>
+      <c r="B21" s="15">
+        <v>20131028</v>
+      </c>
+      <c r="C21" s="15">
+        <v>20131028</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="15">
+        <v>1</v>
+      </c>
+      <c r="F21" s="15">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" t="s">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>13</v>
+      </c>
+      <c r="L21">
+        <v>15</v>
+      </c>
+      <c r="M21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="10"/>
+      <c r="B22" s="15">
+        <v>20131029</v>
+      </c>
+      <c r="C22" s="15">
+        <v>20131030</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="15">
+        <v>21</v>
+      </c>
+      <c r="F22" s="15">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22">
+        <v>13</v>
+      </c>
+      <c r="L22">
+        <v>15</v>
+      </c>
+      <c r="M22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="10"/>
+      <c r="B23" s="15">
+        <v>20131105</v>
+      </c>
+      <c r="C23" s="15">
+        <v>20131106</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="15">
+        <v>22</v>
+      </c>
+      <c r="F23" s="15">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>13</v>
+      </c>
+      <c r="L23">
+        <v>15</v>
+      </c>
+      <c r="M23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="10"/>
+      <c r="B24" s="15">
+        <v>20131108</v>
+      </c>
+      <c r="C24" s="15">
+        <v>20131108</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="15">
+        <v>4</v>
+      </c>
+      <c r="F24" s="15">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24" t="s">
+        <v>5</v>
+      </c>
+      <c r="K24">
+        <v>13</v>
+      </c>
+      <c r="L24">
+        <v>15</v>
+      </c>
+      <c r="M24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="10"/>
+      <c r="B25" s="15">
+        <v>20131110</v>
+      </c>
+      <c r="C25" s="15">
+        <v>20131110</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="15">
+        <v>5</v>
+      </c>
+      <c r="F25" s="15">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" t="s">
+        <v>5</v>
+      </c>
+      <c r="K25">
+        <v>13</v>
+      </c>
+      <c r="L25">
+        <v>15</v>
+      </c>
+      <c r="M25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="10"/>
+      <c r="B26" s="15">
+        <v>20131119</v>
+      </c>
+      <c r="C26" s="15">
+        <v>20131119</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="15">
+        <v>10</v>
+      </c>
+      <c r="F26" s="15">
+        <v>13</v>
+      </c>
+      <c r="G26" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" t="s">
+        <v>5</v>
+      </c>
+      <c r="K26">
+        <v>13</v>
+      </c>
+      <c r="L26">
+        <v>15</v>
+      </c>
+      <c r="M26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="11">
+        <v>2014</v>
+      </c>
+      <c r="B27" s="16">
+        <v>20140107</v>
+      </c>
+      <c r="C27" s="16">
+        <v>20140107</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="16">
+        <v>18</v>
+      </c>
+      <c r="F27" s="16">
+        <v>21</v>
+      </c>
+      <c r="G27" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" t="s">
+        <v>5</v>
+      </c>
+      <c r="K27">
+        <v>13</v>
+      </c>
+      <c r="L27">
+        <v>15</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="11"/>
+      <c r="B28" s="16">
+        <v>20140225</v>
+      </c>
+      <c r="C28" s="16">
+        <v>20140225</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="16">
+        <v>0</v>
+      </c>
+      <c r="F28" s="16">
+        <v>3</v>
+      </c>
+      <c r="G28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28">
+        <v>13</v>
+      </c>
+      <c r="L28">
+        <v>15</v>
+      </c>
+      <c r="M28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="11"/>
+      <c r="B29" s="16">
+        <v>20140329</v>
+      </c>
+      <c r="C29" s="16">
+        <v>20140329</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="16">
+        <v>17</v>
+      </c>
+      <c r="F29" s="16">
+        <v>20</v>
+      </c>
+      <c r="G29" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" t="s">
+        <v>5</v>
+      </c>
+      <c r="K29">
+        <v>13</v>
+      </c>
+      <c r="L29">
+        <v>15</v>
+      </c>
+      <c r="M29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="11"/>
+      <c r="B30" s="16">
+        <v>20140425</v>
+      </c>
+      <c r="C30" s="16">
+        <v>20140425</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="16">
+        <v>0</v>
+      </c>
+      <c r="F30" s="16">
+        <v>3</v>
+      </c>
+      <c r="G30" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" t="s">
+        <v>5</v>
+      </c>
+      <c r="K30">
+        <v>13</v>
+      </c>
+      <c r="L30">
+        <v>15</v>
+      </c>
+      <c r="M30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="11"/>
+      <c r="B31" s="16">
+        <v>20140610</v>
+      </c>
+      <c r="C31" s="16">
+        <v>20140610</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="16">
+        <v>12</v>
+      </c>
+      <c r="F31" s="16">
+        <v>15</v>
+      </c>
+      <c r="G31" t="s">
+        <v>2</v>
+      </c>
+      <c r="H31" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" t="s">
+        <v>4</v>
+      </c>
+      <c r="J31" t="s">
+        <v>5</v>
+      </c>
+      <c r="K31">
+        <v>13</v>
+      </c>
+      <c r="L31">
+        <v>15</v>
+      </c>
+      <c r="M31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="11"/>
+      <c r="B32" s="16">
+        <v>20140610</v>
+      </c>
+      <c r="C32" s="16">
+        <v>20140610</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="16">
+        <v>11</v>
+      </c>
+      <c r="F32" s="16">
+        <v>14</v>
+      </c>
+      <c r="G32" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32" t="s">
+        <v>5</v>
+      </c>
+      <c r="K32">
+        <v>13</v>
+      </c>
+      <c r="L32">
+        <v>15</v>
+      </c>
+      <c r="M32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="11"/>
+      <c r="B33" s="16">
+        <v>20140611</v>
+      </c>
+      <c r="C33" s="16">
+        <v>20140611</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="16">
+        <v>8</v>
+      </c>
+      <c r="F33" s="16">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H33" t="s">
+        <v>3</v>
+      </c>
+      <c r="I33" t="s">
+        <v>4</v>
+      </c>
+      <c r="J33" t="s">
+        <v>5</v>
+      </c>
+      <c r="K33">
+        <v>13</v>
+      </c>
+      <c r="L33">
+        <v>15</v>
+      </c>
+      <c r="M33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="11"/>
+      <c r="B34" s="16">
+        <v>20140910</v>
+      </c>
+      <c r="C34" s="16">
+        <v>20140910</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="16">
+        <v>17</v>
+      </c>
+      <c r="F34" s="16">
+        <v>20</v>
+      </c>
+      <c r="G34" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" t="s">
+        <v>4</v>
+      </c>
+      <c r="J34" t="s">
+        <v>5</v>
+      </c>
+      <c r="K34">
+        <v>13</v>
+      </c>
+      <c r="L34">
+        <v>15</v>
+      </c>
+      <c r="M34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="11"/>
+      <c r="B35" s="16">
+        <v>20141019</v>
+      </c>
+      <c r="C35" s="16">
+        <v>20141019</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="16">
+        <v>4</v>
+      </c>
+      <c r="F35" s="16">
+        <v>7</v>
+      </c>
+      <c r="G35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" t="s">
+        <v>3</v>
+      </c>
+      <c r="I35" t="s">
+        <v>4</v>
+      </c>
+      <c r="J35" t="s">
+        <v>5</v>
+      </c>
+      <c r="K35">
+        <v>13</v>
+      </c>
+      <c r="L35">
+        <v>15</v>
+      </c>
+      <c r="M35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="11"/>
+      <c r="B36" s="16">
+        <v>20141022</v>
+      </c>
+      <c r="C36" s="16">
+        <v>20141022</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="16">
+        <v>14</v>
+      </c>
+      <c r="F36" s="16">
+        <v>17</v>
+      </c>
+      <c r="G36" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" t="s">
+        <v>3</v>
+      </c>
+      <c r="I36" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36" t="s">
+        <v>5</v>
+      </c>
+      <c r="K36">
+        <v>13</v>
+      </c>
+      <c r="L36">
+        <v>15</v>
+      </c>
+      <c r="M36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="11"/>
+      <c r="B37" s="16">
+        <v>20141024</v>
+      </c>
+      <c r="C37" s="16">
+        <v>20141025</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="16">
+        <v>21</v>
+      </c>
+      <c r="F37" s="16">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>2</v>
+      </c>
+      <c r="H37" t="s">
+        <v>3</v>
+      </c>
+      <c r="I37" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" t="s">
+        <v>5</v>
+      </c>
+      <c r="K37">
+        <v>13</v>
+      </c>
+      <c r="L37">
+        <v>15</v>
+      </c>
+      <c r="M37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="11"/>
+      <c r="B38" s="16">
+        <v>20141025</v>
+      </c>
+      <c r="C38" s="16">
+        <v>20141025</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="16">
+        <v>16</v>
+      </c>
+      <c r="F38" s="16">
+        <v>19</v>
+      </c>
+      <c r="G38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H38" t="s">
+        <v>3</v>
+      </c>
+      <c r="I38" t="s">
+        <v>4</v>
+      </c>
+      <c r="J38" t="s">
+        <v>5</v>
+      </c>
+      <c r="K38">
+        <v>13</v>
+      </c>
+      <c r="L38">
+        <v>15</v>
+      </c>
+      <c r="M38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="11"/>
+      <c r="B39" s="16">
+        <v>20141026</v>
+      </c>
+      <c r="C39" s="16">
+        <v>20141026</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="16">
+        <v>10</v>
+      </c>
+      <c r="F39" s="16">
+        <v>13</v>
+      </c>
+      <c r="G39" t="s">
+        <v>2</v>
+      </c>
+      <c r="H39" t="s">
+        <v>3</v>
+      </c>
+      <c r="I39" t="s">
+        <v>4</v>
+      </c>
+      <c r="J39" t="s">
+        <v>5</v>
+      </c>
+      <c r="K39">
+        <v>13</v>
+      </c>
+      <c r="L39">
+        <v>15</v>
+      </c>
+      <c r="M39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="11"/>
+      <c r="B40" s="16">
+        <v>20141027</v>
+      </c>
+      <c r="C40" s="16">
+        <v>20141027</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="16">
+        <v>14</v>
+      </c>
+      <c r="F40" s="16">
+        <v>17</v>
+      </c>
+      <c r="G40" t="s">
+        <v>2</v>
+      </c>
+      <c r="H40" t="s">
+        <v>3</v>
+      </c>
+      <c r="I40" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" t="s">
+        <v>5</v>
+      </c>
+      <c r="K40">
+        <v>13</v>
+      </c>
+      <c r="L40">
+        <v>15</v>
+      </c>
+      <c r="M40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="11"/>
+      <c r="B41" s="16">
+        <v>20141107</v>
+      </c>
+      <c r="C41" s="16">
+        <v>20141107</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="16">
+        <v>16</v>
+      </c>
+      <c r="F41" s="16">
+        <v>19</v>
+      </c>
+      <c r="G41" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" t="s">
+        <v>3</v>
+      </c>
+      <c r="I41" t="s">
+        <v>4</v>
+      </c>
+      <c r="J41" t="s">
+        <v>5</v>
+      </c>
+      <c r="K41">
+        <v>13</v>
+      </c>
+      <c r="L41">
+        <v>15</v>
+      </c>
+      <c r="M41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="11"/>
+      <c r="B42" s="16">
+        <v>20141220</v>
+      </c>
+      <c r="C42" s="16">
+        <v>20141220</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="16">
+        <v>0</v>
+      </c>
+      <c r="F42" s="16">
+        <v>3</v>
+      </c>
+      <c r="G42" t="s">
+        <v>2</v>
+      </c>
+      <c r="H42" t="s">
+        <v>3</v>
+      </c>
+      <c r="I42" t="s">
+        <v>4</v>
+      </c>
+      <c r="J42" t="s">
+        <v>5</v>
+      </c>
+      <c r="K42">
+        <v>13</v>
+      </c>
+      <c r="L42">
+        <v>15</v>
+      </c>
+      <c r="M42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="12">
+        <v>2015</v>
+      </c>
+      <c r="B43" s="17">
+        <v>20150311</v>
+      </c>
+      <c r="C43" s="17">
+        <v>20150311</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="17">
+        <v>16</v>
+      </c>
+      <c r="F43" s="17">
+        <v>19</v>
+      </c>
+      <c r="G43" t="s">
+        <v>2</v>
+      </c>
+      <c r="H43" t="s">
+        <v>3</v>
+      </c>
+      <c r="I43" t="s">
+        <v>4</v>
+      </c>
+      <c r="J43" t="s">
+        <v>5</v>
+      </c>
+      <c r="K43">
+        <v>13</v>
+      </c>
+      <c r="L43">
+        <v>15</v>
+      </c>
+      <c r="M43" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="12"/>
+      <c r="B44" s="17">
+        <v>20150505</v>
+      </c>
+      <c r="C44" s="17">
+        <v>20150506</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="17">
+        <v>22</v>
+      </c>
+      <c r="F44" s="17">
+        <v>1</v>
+      </c>
+      <c r="G44" t="s">
+        <v>2</v>
+      </c>
+      <c r="H44" t="s">
+        <v>3</v>
+      </c>
+      <c r="I44" t="s">
+        <v>4</v>
+      </c>
+      <c r="J44" t="s">
+        <v>5</v>
+      </c>
+      <c r="K44">
+        <v>13</v>
+      </c>
+      <c r="L44">
+        <v>15</v>
+      </c>
+      <c r="M44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A26"/>
+    <mergeCell ref="A27:A42"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="96" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
redone goes detection with 0.20 threshold
</commit_message>
<xml_diff>
--- a/Data/event_list_union.xlsx
+++ b/Data/event_list_union.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9780" yWindow="0" windowWidth="15820" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="GOESPD_0.25" sheetId="1" r:id="rId1"/>
+    <sheet name="GOESPD_0.10" sheetId="3" r:id="rId2"/>
+    <sheet name="XFLR" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="38">
   <si>
     <t>GOES Proton Event Detector List</t>
   </si>
@@ -128,13 +129,19 @@
   </si>
   <si>
     <t>no data in goes</t>
+  </si>
+  <si>
+    <t>Th: 0.25</t>
+  </si>
+  <si>
+    <t>Th: 0.20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -180,6 +187,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="14">
@@ -286,7 +313,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -320,39 +347,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -368,8 +386,60 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -386,6 +456,12 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -402,6 +478,12 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -734,415 +816,834 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="18">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="23">
+        <v>0</v>
+      </c>
+      <c r="C2" s="23">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="4">
+      <c r="D2" s="23">
+        <v>2</v>
+      </c>
+      <c r="E2" s="23">
+        <v>3</v>
+      </c>
+      <c r="F2" s="23">
+        <v>4</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="25">
+        <v>0</v>
+      </c>
+      <c r="J2" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="K2" s="25">
+        <v>2</v>
+      </c>
+      <c r="L2" s="25">
+        <v>3</v>
+      </c>
+      <c r="M2" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="26">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
         <v>20110321</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="H3" s="27">
+        <v>1</v>
+      </c>
+      <c r="I3" s="17">
+        <v>20110321</v>
+      </c>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="26">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
         <v>20110607</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>20110608</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="H4" s="27">
+        <v>2</v>
+      </c>
+      <c r="I4" s="17">
+        <v>20110607</v>
+      </c>
+      <c r="J4" s="17">
+        <v>20110608</v>
+      </c>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="26">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
         <v>20110804</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="27">
+        <v>3</v>
+      </c>
+      <c r="I5" s="17">
+        <v>20110804</v>
+      </c>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="26">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
         <v>20110809</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="4">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="H6" s="27">
+        <v>4</v>
+      </c>
+      <c r="I6" s="17">
+        <v>20110809</v>
+      </c>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="26">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
         <v>20110907</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="H7" s="27">
+        <v>5</v>
+      </c>
+      <c r="I7" s="17">
+        <v>20110907</v>
+      </c>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="26">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>20120123</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>20120124</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="H8" s="28">
+        <v>6</v>
+      </c>
+      <c r="I8" s="18">
+        <v>20110923</v>
+      </c>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="26">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
         <v>20120127</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>20120128</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>20120129</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="4">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="H9" s="27">
+        <v>7</v>
+      </c>
+      <c r="I9" s="17">
+        <v>20120123</v>
+      </c>
+      <c r="J9" s="17">
+        <v>20120124</v>
+      </c>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="26">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>20120307</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>20120308</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>20120309</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>20120310</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>20120311</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4">
+      <c r="H10" s="27">
+        <v>8</v>
+      </c>
+      <c r="I10" s="17">
+        <v>20120127</v>
+      </c>
+      <c r="J10" s="17">
+        <v>20120128</v>
+      </c>
+      <c r="K10" s="17">
+        <v>20120129</v>
+      </c>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="26">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>20120313</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>20120314</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="4">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="H11" s="27">
+        <v>9</v>
+      </c>
+      <c r="I11" s="17">
+        <v>20120307</v>
+      </c>
+      <c r="J11" s="17">
+        <v>20120308</v>
+      </c>
+      <c r="K11" s="17">
+        <v>20120309</v>
+      </c>
+      <c r="L11" s="17">
+        <v>20120310</v>
+      </c>
+      <c r="M11" s="17">
+        <v>20120311</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="26">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>20120517</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>20120518</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="H12" s="27">
+        <v>10</v>
+      </c>
+      <c r="I12" s="17">
+        <v>20120313</v>
+      </c>
+      <c r="J12" s="17">
+        <v>20120314</v>
+      </c>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="26">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>20120707</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>20120708</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>20120709</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="4">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="H13" s="27">
+        <v>11</v>
+      </c>
+      <c r="I13" s="17">
+        <v>20120517</v>
+      </c>
+      <c r="J13" s="17">
+        <v>20120518</v>
+      </c>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="26">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>20120712</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="4">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="H14" s="27">
+        <v>12</v>
+      </c>
+      <c r="I14" s="17">
+        <v>20120707</v>
+      </c>
+      <c r="J14" s="17">
+        <v>20120708</v>
+      </c>
+      <c r="K14" s="17">
+        <v>20120709</v>
+      </c>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="26">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
         <v>20120719</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="4">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="H15" s="27">
+        <v>13</v>
+      </c>
+      <c r="I15" s="17">
+        <v>20120712</v>
+      </c>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="26">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>20120723</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>20120724</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>20120725</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="4">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="H16" s="27">
+        <v>14</v>
+      </c>
+      <c r="I16" s="17">
+        <v>20120719</v>
+      </c>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="26">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
         <v>20130411</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>20130412</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="4">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="H17" s="27">
+        <v>15</v>
+      </c>
+      <c r="I17" s="17">
+        <v>20120723</v>
+      </c>
+      <c r="J17" s="17">
+        <v>20120724</v>
+      </c>
+      <c r="K17" s="17">
+        <v>20120725</v>
+      </c>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="26">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>20130522</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>20130523</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>20130524</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="4">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="H18" s="28">
+        <v>16</v>
+      </c>
+      <c r="I18" s="18">
+        <v>20120928</v>
+      </c>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="26">
         <v>17</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>20131102</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="4">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="H19" s="27">
+        <v>17</v>
+      </c>
+      <c r="I19" s="17">
+        <v>20130411</v>
+      </c>
+      <c r="J19" s="17">
+        <v>20130412</v>
+      </c>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="26">
         <v>18</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>20131228</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="4">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="H20" s="27">
+        <v>18</v>
+      </c>
+      <c r="I20" s="17">
+        <v>20130522</v>
+      </c>
+      <c r="J20" s="17">
+        <v>20130523</v>
+      </c>
+      <c r="K20" s="17">
+        <v>20130524</v>
+      </c>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="26">
         <v>19</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>20140106</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>20140107</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>20140108</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>20140109</v>
       </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="4">
+      <c r="F21" s="1"/>
+      <c r="H21" s="27">
+        <v>19</v>
+      </c>
+      <c r="I21" s="17">
+        <v>20131102</v>
+      </c>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="26">
         <v>20</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>20140220</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="4">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="H22" s="27">
+        <v>20</v>
+      </c>
+      <c r="I22" s="17">
+        <v>20131228</v>
+      </c>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="26">
         <v>21</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>20140225</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>20140226</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>20140227</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="4">
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="H23" s="27">
+        <v>21</v>
+      </c>
+      <c r="I23" s="17">
+        <v>20140106</v>
+      </c>
+      <c r="J23" s="17">
+        <v>20140107</v>
+      </c>
+      <c r="K23" s="17">
+        <v>20140108</v>
+      </c>
+      <c r="L23" s="17">
+        <v>20140109</v>
+      </c>
+      <c r="M23" s="17"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="26">
         <v>22</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>20140418</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="4">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="H24" s="27">
+        <v>22</v>
+      </c>
+      <c r="I24" s="17">
+        <v>20140220</v>
+      </c>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="26">
         <v>23</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>20140902</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>20140903</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>20140904</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>20140905</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="1">
         <v>20140906</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="4">
+      <c r="H25" s="27">
+        <v>23</v>
+      </c>
+      <c r="I25" s="17">
+        <v>20140225</v>
+      </c>
+      <c r="J25" s="17">
+        <v>20140226</v>
+      </c>
+      <c r="K25" s="17">
+        <v>20140227</v>
+      </c>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="26">
         <v>24</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>20140910</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>20140911</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="4">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="H26" s="27">
+        <v>24</v>
+      </c>
+      <c r="I26" s="17">
+        <v>20140418</v>
+      </c>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="26">
         <v>25</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>20151029</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="4">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="H27" s="27">
+        <v>25</v>
+      </c>
+      <c r="I27" s="17">
+        <v>20140902</v>
+      </c>
+      <c r="J27" s="17">
+        <v>20140903</v>
+      </c>
+      <c r="K27" s="17">
+        <v>20140904</v>
+      </c>
+      <c r="L27" s="17">
+        <v>20140905</v>
+      </c>
+      <c r="M27" s="17">
+        <v>20140906</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="26">
         <v>26</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>20170906</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="H28" s="27">
+        <v>26</v>
+      </c>
+      <c r="I28" s="17">
+        <v>20140910</v>
+      </c>
+      <c r="J28" s="17">
+        <v>20140911</v>
+      </c>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="26">
+        <v>27</v>
+      </c>
+      <c r="B29" s="17">
+        <v>20170910</v>
+      </c>
+      <c r="C29" s="17">
+        <v>20170911</v>
+      </c>
+      <c r="D29" s="17">
+        <v>20170912</v>
+      </c>
+      <c r="E29" s="17">
+        <v>20170913</v>
+      </c>
+      <c r="F29" s="17">
+        <v>20170914</v>
+      </c>
+      <c r="H29" s="27">
+        <v>27</v>
+      </c>
+      <c r="I29" s="17">
+        <v>20151029</v>
+      </c>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="H30" s="27">
+        <v>28</v>
+      </c>
+      <c r="I30" s="17">
+        <v>20170906</v>
+      </c>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="H31" s="28">
+        <v>29</v>
+      </c>
+      <c r="I31" s="18">
+        <v>20170908</v>
+      </c>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="H32" s="27">
+        <v>30</v>
+      </c>
+      <c r="I32" s="17">
+        <v>20170910</v>
+      </c>
+      <c r="J32" s="17">
+        <v>20170911</v>
+      </c>
+      <c r="K32" s="17">
+        <v>20170912</v>
+      </c>
+      <c r="L32" s="17">
+        <v>20170913</v>
+      </c>
+      <c r="M32" s="17">
+        <v>20170914</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:M1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="59" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -1153,69 +1654,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:14" ht="18">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="8">
+      <c r="A3" s="13">
         <v>2011</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="6">
         <v>20110309</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="6">
         <v>20110310</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="6">
         <v>23</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="6">
         <v>2</v>
       </c>
       <c r="G3" t="s">
@@ -1236,25 +1758,25 @@
       <c r="L3">
         <v>15</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="8"/>
-      <c r="B4" s="13">
+      <c r="A4" s="13"/>
+      <c r="B4" s="6">
         <v>20110809</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="6">
         <v>20110809</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="13">
-        <v>7</v>
-      </c>
-      <c r="F4" s="13">
+      <c r="E4" s="6">
+        <v>7</v>
+      </c>
+      <c r="F4" s="6">
         <v>10</v>
       </c>
       <c r="G4" t="s">
@@ -1280,20 +1802,20 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="8"/>
-      <c r="B5" s="13">
+      <c r="A5" s="13"/>
+      <c r="B5" s="6">
         <v>20110906</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="6">
         <v>20110907</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="6">
         <v>22</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="6">
         <v>1</v>
       </c>
       <c r="G5" t="s">
@@ -1319,20 +1841,20 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="8"/>
-      <c r="B6" s="13">
+      <c r="A6" s="13"/>
+      <c r="B6" s="6">
         <v>20110922</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="6">
         <v>20110922</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="6">
         <v>10</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="6">
         <v>13</v>
       </c>
       <c r="G6" t="s">
@@ -1358,20 +1880,20 @@
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="8"/>
-      <c r="B7" s="13">
+      <c r="A7" s="13"/>
+      <c r="B7" s="6">
         <v>20110924</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="6">
         <v>20110924</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="6">
         <v>9</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="6">
         <v>12</v>
       </c>
       <c r="G7" t="s">
@@ -1397,20 +1919,20 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="8"/>
-      <c r="B8" s="13">
+      <c r="A8" s="13"/>
+      <c r="B8" s="6">
         <v>20111103</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="6">
         <v>20111103</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="6">
         <v>20</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="6">
         <v>23</v>
       </c>
       <c r="G8" t="s">
@@ -1436,22 +1958,22 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="9">
+      <c r="A9" s="14">
         <v>2012</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="7">
         <v>20120127</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="7">
         <v>20120127</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="7">
         <v>17</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="7">
         <v>20</v>
       </c>
       <c r="G9" t="s">
@@ -1472,25 +1994,25 @@
       <c r="L9">
         <v>15</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="9"/>
-      <c r="B10" s="14">
+      <c r="A10" s="14"/>
+      <c r="B10" s="7">
         <v>20120307</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="7">
         <v>20120307</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="7">
         <v>0</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="7">
         <v>3</v>
       </c>
       <c r="G10" t="s">
@@ -1516,20 +2038,20 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="9"/>
-      <c r="B11" s="14">
+      <c r="A11" s="14"/>
+      <c r="B11" s="7">
         <v>20120307</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="7">
         <v>20120307</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="14">
+      <c r="D11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="7">
         <v>0</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="7">
         <v>3</v>
       </c>
       <c r="G11" t="s">
@@ -1555,20 +2077,20 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="9"/>
-      <c r="B12" s="14">
+      <c r="A12" s="14"/>
+      <c r="B12" s="7">
         <v>20120706</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="7">
         <v>20120707</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="7">
         <v>23</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="7">
         <v>2</v>
       </c>
       <c r="G12" t="s">
@@ -1594,20 +2116,20 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="9"/>
-      <c r="B13" s="14">
+      <c r="A13" s="14"/>
+      <c r="B13" s="7">
         <v>20120712</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="7">
         <v>20120712</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="14">
-        <v>15</v>
-      </c>
-      <c r="F13" s="14">
+      <c r="E13" s="7">
+        <v>15</v>
+      </c>
+      <c r="F13" s="7">
         <v>18</v>
       </c>
       <c r="G13" t="s">
@@ -1633,20 +2155,20 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="9"/>
-      <c r="B14" s="14">
+      <c r="A14" s="14"/>
+      <c r="B14" s="7">
         <v>20121023</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="7">
         <v>20121023</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="14">
-        <v>3</v>
-      </c>
-      <c r="F14" s="14">
+      <c r="D14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="7">
+        <v>3</v>
+      </c>
+      <c r="F14" s="7">
         <v>6</v>
       </c>
       <c r="G14" t="s">
@@ -1672,22 +2194,22 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="10">
+      <c r="A15" s="15">
         <v>2013</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="8">
         <v>20130513</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="8">
         <v>20130513</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="8">
         <v>1</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="8">
         <v>4</v>
       </c>
       <c r="G15" t="s">
@@ -1708,28 +2230,28 @@
       <c r="L15">
         <v>15</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="M15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N15" s="7" t="s">
+      <c r="N15" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="10"/>
-      <c r="B16" s="15">
+      <c r="A16" s="15"/>
+      <c r="B16" s="8">
         <v>20130513</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="8">
         <v>20130513</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="15">
-        <v>15</v>
-      </c>
-      <c r="F16" s="15">
+      <c r="E16" s="8">
+        <v>15</v>
+      </c>
+      <c r="F16" s="8">
         <v>18</v>
       </c>
       <c r="G16" t="s">
@@ -1750,28 +2272,28 @@
       <c r="L16">
         <v>15</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="M16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N16" s="7" t="s">
+      <c r="N16" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="10"/>
-      <c r="B17" s="15">
+      <c r="A17" s="15"/>
+      <c r="B17" s="8">
         <v>20130514</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="8">
         <v>20130514</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="8">
         <v>0</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="8">
         <v>3</v>
       </c>
       <c r="G17" t="s">
@@ -1797,20 +2319,20 @@
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="10"/>
-      <c r="B18" s="15">
+      <c r="A18" s="15"/>
+      <c r="B18" s="8">
         <v>20130515</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="8">
         <v>20130515</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="8">
         <v>1</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="8">
         <v>4</v>
       </c>
       <c r="G18" t="s">
@@ -1831,28 +2353,28 @@
       <c r="L18">
         <v>15</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="M18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N18" s="7" t="s">
+      <c r="N18" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="10"/>
-      <c r="B19" s="15">
+      <c r="A19" s="15"/>
+      <c r="B19" s="8">
         <v>20131025</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="8">
         <v>20131025</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="15">
-        <v>7</v>
-      </c>
-      <c r="F19" s="15">
+      <c r="E19" s="8">
+        <v>7</v>
+      </c>
+      <c r="F19" s="8">
         <v>10</v>
       </c>
       <c r="G19" t="s">
@@ -1878,20 +2400,20 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="10"/>
-      <c r="B20" s="15">
+      <c r="A20" s="15"/>
+      <c r="B20" s="8">
         <v>20131025</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="8">
         <v>20131025</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="8">
         <v>14</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="8">
         <v>17</v>
       </c>
       <c r="G20" t="s">
@@ -1917,20 +2439,20 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="10"/>
-      <c r="B21" s="15">
+      <c r="A21" s="15"/>
+      <c r="B21" s="8">
         <v>20131028</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="8">
         <v>20131028</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="8">
         <v>1</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="8">
         <v>4</v>
       </c>
       <c r="G21" t="s">
@@ -1956,20 +2478,20 @@
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="10"/>
-      <c r="B22" s="15">
+      <c r="A22" s="15"/>
+      <c r="B22" s="8">
         <v>20131029</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="8">
         <v>20131030</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="8">
         <v>21</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="8">
         <v>0</v>
       </c>
       <c r="G22" t="s">
@@ -1995,20 +2517,20 @@
       </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="10"/>
-      <c r="B23" s="15">
+      <c r="A23" s="15"/>
+      <c r="B23" s="8">
         <v>20131105</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="8">
         <v>20131106</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="8">
         <v>22</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="8">
         <v>1</v>
       </c>
       <c r="G23" t="s">
@@ -2034,20 +2556,20 @@
       </c>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="10"/>
-      <c r="B24" s="15">
+      <c r="A24" s="15"/>
+      <c r="B24" s="8">
         <v>20131108</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="8">
         <v>20131108</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="15">
-        <v>4</v>
-      </c>
-      <c r="F24" s="15">
+      <c r="E24" s="8">
+        <v>4</v>
+      </c>
+      <c r="F24" s="8">
         <v>7</v>
       </c>
       <c r="G24" t="s">
@@ -2073,20 +2595,20 @@
       </c>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="10"/>
-      <c r="B25" s="15">
+      <c r="A25" s="15"/>
+      <c r="B25" s="8">
         <v>20131110</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="8">
         <v>20131110</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="15">
-        <v>5</v>
-      </c>
-      <c r="F25" s="15">
+      <c r="E25" s="8">
+        <v>5</v>
+      </c>
+      <c r="F25" s="8">
         <v>8</v>
       </c>
       <c r="G25" t="s">
@@ -2112,20 +2634,20 @@
       </c>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="10"/>
-      <c r="B26" s="15">
+      <c r="A26" s="15"/>
+      <c r="B26" s="8">
         <v>20131119</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="8">
         <v>20131119</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="8">
         <v>10</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="8">
         <v>13</v>
       </c>
       <c r="G26" t="s">
@@ -2151,22 +2673,22 @@
       </c>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="11">
+      <c r="A27" s="16">
         <v>2014</v>
       </c>
-      <c r="B27" s="16">
+      <c r="B27" s="9">
         <v>20140107</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="9">
         <v>20140107</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="9">
         <v>18</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="9">
         <v>21</v>
       </c>
       <c r="G27" t="s">
@@ -2187,25 +2709,25 @@
       <c r="L27">
         <v>15</v>
       </c>
-      <c r="M27" s="5" t="s">
+      <c r="M27" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="11"/>
-      <c r="B28" s="16">
+      <c r="A28" s="16"/>
+      <c r="B28" s="9">
         <v>20140225</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="9">
         <v>20140225</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="9">
         <v>0</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="9">
         <v>3</v>
       </c>
       <c r="G28" t="s">
@@ -2231,20 +2753,20 @@
       </c>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="11"/>
-      <c r="B29" s="16">
+      <c r="A29" s="16"/>
+      <c r="B29" s="9">
         <v>20140329</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="9">
         <v>20140329</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="9">
         <v>17</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="9">
         <v>20</v>
       </c>
       <c r="G29" t="s">
@@ -2270,20 +2792,20 @@
       </c>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="11"/>
-      <c r="B30" s="16">
+      <c r="A30" s="16"/>
+      <c r="B30" s="9">
         <v>20140425</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="9">
         <v>20140425</v>
       </c>
-      <c r="D30" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="16">
+      <c r="D30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="9">
         <v>0</v>
       </c>
-      <c r="F30" s="16">
+      <c r="F30" s="9">
         <v>3</v>
       </c>
       <c r="G30" t="s">
@@ -2309,20 +2831,20 @@
       </c>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="11"/>
-      <c r="B31" s="16">
+      <c r="A31" s="16"/>
+      <c r="B31" s="9">
         <v>20140610</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="9">
         <v>20140610</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E31" s="16">
+      <c r="E31" s="9">
         <v>12</v>
       </c>
-      <c r="F31" s="16">
+      <c r="F31" s="9">
         <v>15</v>
       </c>
       <c r="G31" t="s">
@@ -2348,20 +2870,20 @@
       </c>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="11"/>
-      <c r="B32" s="16">
+      <c r="A32" s="16"/>
+      <c r="B32" s="9">
         <v>20140610</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C32" s="9">
         <v>20140610</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="16">
+      <c r="E32" s="9">
         <v>11</v>
       </c>
-      <c r="F32" s="16">
+      <c r="F32" s="9">
         <v>14</v>
       </c>
       <c r="G32" t="s">
@@ -2387,20 +2909,20 @@
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="11"/>
-      <c r="B33" s="16">
+      <c r="A33" s="16"/>
+      <c r="B33" s="9">
         <v>20140611</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="9">
         <v>20140611</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="16">
+      <c r="E33" s="9">
         <v>8</v>
       </c>
-      <c r="F33" s="16">
+      <c r="F33" s="9">
         <v>11</v>
       </c>
       <c r="G33" t="s">
@@ -2426,20 +2948,20 @@
       </c>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="11"/>
-      <c r="B34" s="16">
+      <c r="A34" s="16"/>
+      <c r="B34" s="9">
         <v>20140910</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="9">
         <v>20140910</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="9">
         <v>17</v>
       </c>
-      <c r="F34" s="16">
+      <c r="F34" s="9">
         <v>20</v>
       </c>
       <c r="G34" t="s">
@@ -2465,20 +2987,20 @@
       </c>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="11"/>
-      <c r="B35" s="16">
+      <c r="A35" s="16"/>
+      <c r="B35" s="9">
         <v>20141019</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C35" s="9">
         <v>20141019</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="16">
-        <v>4</v>
-      </c>
-      <c r="F35" s="16">
+      <c r="E35" s="9">
+        <v>4</v>
+      </c>
+      <c r="F35" s="9">
         <v>7</v>
       </c>
       <c r="G35" t="s">
@@ -2504,20 +3026,20 @@
       </c>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="11"/>
-      <c r="B36" s="16">
+      <c r="A36" s="16"/>
+      <c r="B36" s="9">
         <v>20141022</v>
       </c>
-      <c r="C36" s="16">
+      <c r="C36" s="9">
         <v>20141022</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E36" s="16">
+      <c r="E36" s="9">
         <v>14</v>
       </c>
-      <c r="F36" s="16">
+      <c r="F36" s="9">
         <v>17</v>
       </c>
       <c r="G36" t="s">
@@ -2543,20 +3065,20 @@
       </c>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="11"/>
-      <c r="B37" s="16">
+      <c r="A37" s="16"/>
+      <c r="B37" s="9">
         <v>20141024</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37" s="9">
         <v>20141025</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="16">
+      <c r="E37" s="9">
         <v>21</v>
       </c>
-      <c r="F37" s="16">
+      <c r="F37" s="9">
         <v>0</v>
       </c>
       <c r="G37" t="s">
@@ -2582,20 +3104,20 @@
       </c>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="11"/>
-      <c r="B38" s="16">
+      <c r="A38" s="16"/>
+      <c r="B38" s="9">
         <v>20141025</v>
       </c>
-      <c r="C38" s="16">
+      <c r="C38" s="9">
         <v>20141025</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="16">
+      <c r="E38" s="9">
         <v>16</v>
       </c>
-      <c r="F38" s="16">
+      <c r="F38" s="9">
         <v>19</v>
       </c>
       <c r="G38" t="s">
@@ -2621,20 +3143,20 @@
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="11"/>
-      <c r="B39" s="16">
+      <c r="A39" s="16"/>
+      <c r="B39" s="9">
         <v>20141026</v>
       </c>
-      <c r="C39" s="16">
+      <c r="C39" s="9">
         <v>20141026</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E39" s="16">
+      <c r="E39" s="9">
         <v>10</v>
       </c>
-      <c r="F39" s="16">
+      <c r="F39" s="9">
         <v>13</v>
       </c>
       <c r="G39" t="s">
@@ -2660,20 +3182,20 @@
       </c>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="11"/>
-      <c r="B40" s="16">
+      <c r="A40" s="16"/>
+      <c r="B40" s="9">
         <v>20141027</v>
       </c>
-      <c r="C40" s="16">
+      <c r="C40" s="9">
         <v>20141027</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="16">
+      <c r="E40" s="9">
         <v>14</v>
       </c>
-      <c r="F40" s="16">
+      <c r="F40" s="9">
         <v>17</v>
       </c>
       <c r="G40" t="s">
@@ -2699,20 +3221,20 @@
       </c>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="11"/>
-      <c r="B41" s="16">
+      <c r="A41" s="16"/>
+      <c r="B41" s="9">
         <v>20141107</v>
       </c>
-      <c r="C41" s="16">
+      <c r="C41" s="9">
         <v>20141107</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="16">
+      <c r="E41" s="9">
         <v>16</v>
       </c>
-      <c r="F41" s="16">
+      <c r="F41" s="9">
         <v>19</v>
       </c>
       <c r="G41" t="s">
@@ -2738,20 +3260,20 @@
       </c>
     </row>
     <row r="42" spans="1:13">
-      <c r="A42" s="11"/>
-      <c r="B42" s="16">
+      <c r="A42" s="16"/>
+      <c r="B42" s="9">
         <v>20141220</v>
       </c>
-      <c r="C42" s="16">
+      <c r="C42" s="9">
         <v>20141220</v>
       </c>
-      <c r="D42" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="16">
+      <c r="D42" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="9">
         <v>0</v>
       </c>
-      <c r="F42" s="16">
+      <c r="F42" s="9">
         <v>3</v>
       </c>
       <c r="G42" t="s">
@@ -2780,19 +3302,19 @@
       <c r="A43" s="12">
         <v>2015</v>
       </c>
-      <c r="B43" s="17">
+      <c r="B43" s="10">
         <v>20150311</v>
       </c>
-      <c r="C43" s="17">
+      <c r="C43" s="10">
         <v>20150311</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="17">
+      <c r="E43" s="10">
         <v>16</v>
       </c>
-      <c r="F43" s="17">
+      <c r="F43" s="10">
         <v>19</v>
       </c>
       <c r="G43" t="s">
@@ -2813,25 +3335,25 @@
       <c r="L43">
         <v>15</v>
       </c>
-      <c r="M43" s="5" t="s">
+      <c r="M43" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="12"/>
-      <c r="B44" s="17">
+      <c r="B44" s="10">
         <v>20150505</v>
       </c>
-      <c r="C44" s="17">
+      <c r="C44" s="10">
         <v>20150506</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="17">
+      <c r="E44" s="10">
         <v>22</v>
       </c>
-      <c r="F44" s="17">
+      <c r="F44" s="10">
         <v>1</v>
       </c>
       <c r="G44" t="s">
@@ -2867,7 +3389,7 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="96" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="51" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>